<commit_message>
[Manish] Added: Refactor code
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/fb/keyword/scenerios/KeywordDrivenData.xlsx
+++ b/src/main/java/com/qa/fb/keyword/scenerios/KeywordDrivenData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -101,9 +101,6 @@
     <t>chrome</t>
   </si>
   <si>
-    <t>manishkumar0156@gmail.com</t>
-  </si>
-  <si>
     <t>behappy@</t>
   </si>
   <si>
@@ -195,6 +192,9 @@
   </si>
   <si>
     <t>//button[contains(text(),'Sign Up')]</t>
+  </si>
+  <si>
+    <t>manish@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -678,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -695,7 +695,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -828,13 +828,13 @@
     </row>
     <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>31</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="D4" s="11" t="s">
         <v>20</v>
@@ -845,98 +845,98 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>20</v>
@@ -947,30 +947,30 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="14" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D12" s="14" t="s">
         <v>20</v>
@@ -981,30 +981,30 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B14" s="13" t="s">
         <v>22</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>20</v>
@@ -1015,7 +1015,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>6</v>

</xml_diff>